<commit_message>
added register page and minor changes in existing code
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D44E620-E29F-447F-A11F-B684D9430443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC13AD2B-ED57-4A9F-8614-B6B509064C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>testname</t>
   </si>
@@ -82,13 +82,22 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Checkouting the adidas shoes from NOP commerece</t>
+  </si>
+  <si>
+    <t>Registering in NOP Commerce site</t>
+  </si>
+  <si>
+    <t>nopRegisterTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,20 +108,6 @@
     <font>
       <sz val="22"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,24 +137,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,14 +520,14 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -546,11 +537,11 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -559,6 +550,23 @@
         <v>6</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -570,10 +578,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +622,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -640,7 +648,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -666,158 +674,28 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>9</v>
+      <c r="A4" s="5" t="s">
+        <v>24</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -825,8 +703,9 @@
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{DCC12871-E981-4C68-BE2E-90EB6CFBAFCF}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{5AC53084-F0CD-47A9-8536-DAD43832629F}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{F2FE6203-C33F-4238-ABE5-340C511F1521}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
minor changed done in cell phone check out test
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3300564E-30AE-42DD-8BDF-8B89C0112E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D797C20-DB5A-48C9-B074-069D6676404D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="1" r:id="rId1"/>
@@ -93,10 +93,10 @@
     <t>nopRegisterTest</t>
   </si>
   <si>
-    <t>NokiaCellPhoneCheckoutTest</t>
-  </si>
-  <si>
     <t>Checkouting the Nokia Cellphone from NOP commerece</t>
+  </si>
+  <si>
+    <t>nokiaCellPhoneCheckoutTest</t>
   </si>
 </sst>
 </file>
@@ -173,9 +173,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -213,9 +213,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -248,9 +248,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -283,9 +300,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -461,20 +495,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51.109375" customWidth="1"/>
-    <col min="2" max="2" width="107.33203125" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="51.140625" customWidth="1"/>
+    <col min="2" max="2" width="107.28515625" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -491,7 +525,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -508,7 +542,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -525,7 +559,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -542,12 +576,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -569,22 +603,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.44140625" customWidth="1"/>
-    <col min="2" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="28.5546875" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="59.5546875" customWidth="1"/>
+    <col min="1" max="1" width="50.42578125" customWidth="1"/>
+    <col min="2" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -610,7 +644,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" ht="34.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
@@ -636,7 +670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -662,7 +696,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>24</v>
       </c>
@@ -688,9 +722,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>

</xml_diff>